<commit_message>
1st Try to adjust Fig4s
1. Seems fold_tl_tko is enough
2. Change secretion into enzymatic reaction cause problem of the
secretion profile. Linear increase instead.
3. Will delete the mistake files generated after changing the enzymatic
secretion
4. Will go back to simple profiles to justify the need of fold in tl or
secretion.
</commit_message>
<xml_diff>
--- a/doc/reaction_table.xlsx
+++ b/doc/reaction_table.xlsx
@@ -3364,9 +3364,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{A9AEF393-04AA-5841-B838-22F3B63C300E}" name="zhang Cheng" id="-845660997" dateTime="2014-04-10T23:04:20"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>